<commit_message>
Sol grafica, escaleta y guion actual cn _06_10
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion10/ES_CN_06_10_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion10/ES_CN_06_10_CO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8730"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
-    <sheet name="DATOS" sheetId="1" r:id="rId2"/>
+    <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -16,12 +16,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$M$2:$N$30</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="239">
   <si>
     <t>Asignatura</t>
   </si>
@@ -456,12 +456,6 @@
     <t>FQ_09_02</t>
   </si>
   <si>
-    <t xml:space="preserve">Autoevaluación características atómicas  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contiene una autoevaluación para evaluar tus conocimientos aprendidos de la materia y sus propiedades. </t>
-  </si>
-  <si>
     <t>Recurso M4A-01</t>
   </si>
   <si>
@@ -478,9 +472,6 @@
   </si>
   <si>
     <t xml:space="preserve">La historia de los modelos atómicos </t>
-  </si>
-  <si>
-    <t>Webquest pensada para profundizar en la evolución de los modelos atómicos a lo largo de la historia</t>
   </si>
   <si>
     <t>La historia de los modelos atómicos</t>
@@ -608,12 +599,6 @@
     <t>Recurso M2A-03</t>
   </si>
   <si>
-    <t>Autoevaluación de los modelos atómicos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contiene una autoevaluación para evaluar tus conocimientos aprendidos de los modelos atómicos. </t>
-  </si>
-  <si>
     <t xml:space="preserve">El modelo atómico actual </t>
   </si>
   <si>
@@ -701,9 +686,6 @@
     <t xml:space="preserve">Actividad que propone realizar la construcción de modelos para comprender la evolución de los conocimientos sobre el átomo </t>
   </si>
   <si>
-    <t xml:space="preserve">Competencias :modelo atómico actual </t>
-  </si>
-  <si>
     <t xml:space="preserve">Actividad que propone realizar una representación del modelo actual usando diferentes materiales </t>
   </si>
   <si>
@@ -713,12 +695,6 @@
     <t>Recurso M102AB-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Autoevaluación  de la materia y sus propiedades </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contiene una autoevaluación para evaluar tus conocimientos aprendidos de la materia y sus propiedades </t>
-  </si>
-  <si>
     <t>Recurso M4A-02</t>
   </si>
   <si>
@@ -734,9 +710,6 @@
     <t xml:space="preserve">Mapa conceptual </t>
   </si>
   <si>
-    <t xml:space="preserve">Mapa conceptual del átomo </t>
-  </si>
-  <si>
     <t xml:space="preserve">Banco de actividades:el átomo </t>
   </si>
   <si>
@@ -750,13 +723,40 @@
   </si>
   <si>
     <t>Recurso M101A-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las características atómicas  </t>
+  </si>
+  <si>
+    <t>Actividad que permite reconocer lo aprendido acerca de la materia y sus propiedades</t>
+  </si>
+  <si>
+    <t>Interactivo que permite profundizar en la evolución de los modelos atómicos a lo largo de la historia</t>
+  </si>
+  <si>
+    <t>Actividad que permite verificar que has aprendido acerca de los modelos atómicos</t>
+  </si>
+  <si>
+    <t>¿Qué tanto sabes de los modelos atómicos?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Competencias: modelo atómico actual </t>
+  </si>
+  <si>
+    <t>Evaluación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evalúa tus conocimientos sobre el tema El átomo </t>
+  </si>
+  <si>
+    <t>Mapa conceptual del tema El átomo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -800,8 +800,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -886,8 +893,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -964,11 +977,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1024,34 +1046,60 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1091,6 +1139,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1414,9 +1480,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K27" sqref="A27:XFD27"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,16 +1491,16 @@
     <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="25.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" customWidth="1"/>
     <col min="13" max="14" width="9.28515625" customWidth="1"/>
-    <col min="15" max="15" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" style="1" customWidth="1"/>
     <col min="16" max="16" width="16.5703125" style="1" customWidth="1"/>
     <col min="17" max="17" width="20.42578125" style="1" customWidth="1"/>
     <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
@@ -1444,152 +1510,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="24" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="29" t="s">
+      <c r="N1" s="73"/>
+      <c r="O1" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="61" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="Q1" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="R1" s="80" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="31" t="s">
+      <c r="S1" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="T1" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="31" t="s">
+      <c r="U1" s="76" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="24" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="44"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="68"/>
       <c r="M2" s="25" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="32"/>
-    </row>
-    <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="77"/>
+    </row>
+    <row r="3" spans="1:21" s="55" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="53" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="H3" s="9">
+      <c r="F3" s="53"/>
+      <c r="G3" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="53">
         <v>1</v>
       </c>
-      <c r="I3" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="23"/>
-      <c r="P3" s="9" t="s">
+      <c r="I3" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="10">
-        <v>6</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="S3" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="T3" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>130</v>
+      <c r="J3" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="K3" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="P3" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="R3" s="53" t="s">
+        <v>140</v>
+      </c>
+      <c r="S3" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="T3" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="U3" s="53" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1606,32 +1672,32 @@
         <v>124</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="F4" s="9"/>
+        <v>125</v>
+      </c>
+      <c r="F4" s="27"/>
       <c r="G4" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H4" s="9">
         <v>2</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="19" t="s">
         <v>20</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="K4" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="K4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="9"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="23"/>
       <c r="P4" s="9" t="s">
         <v>19</v>
       </c>
@@ -1645,7 +1711,7 @@
         <v>128</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="U4" s="10" t="s">
         <v>130</v>
@@ -1669,45 +1735,45 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H5" s="9">
         <v>3</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="9" t="s">
-        <v>138</v>
-      </c>
+      <c r="N5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="9"/>
       <c r="P5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="10" t="s">
-        <v>139</v>
+      <c r="Q5" s="10">
+        <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1727,8 +1793,8 @@
         <v>131</v>
       </c>
       <c r="F6" s="9"/>
-      <c r="G6" s="16" t="s">
-        <v>144</v>
+      <c r="G6" s="57" t="s">
+        <v>230</v>
       </c>
       <c r="H6" s="9">
         <v>4</v>
@@ -1736,8 +1802,8 @@
       <c r="I6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="17" t="s">
-        <v>145</v>
+      <c r="J6" s="56" t="s">
+        <v>231</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1763,123 +1829,123 @@
         <v>128</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U6" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:21" s="51" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="16" t="s">
+      <c r="E7" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="F7" s="41"/>
+      <c r="G7" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" s="41">
+        <v>5</v>
+      </c>
+      <c r="I7" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="K7" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="R7" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="S7" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="T7" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="H7" s="9">
-        <v>5</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q7" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="R7" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="S7" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="T7" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="U7" s="10" t="s">
+      <c r="U7" s="48" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="23">
+        <v>6</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="R8" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="S8" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="T8" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="H8" s="9">
-        <v>6</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="P8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q8" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="R8" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="S8" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="T8" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="U8" s="10" t="s">
+      <c r="U8" s="34" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1894,16 +1960,16 @@
         <v>123</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H9" s="9">
         <v>7</v>
@@ -1912,7 +1978,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>20</v>
@@ -1938,7 +2004,7 @@
         <v>128</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="U9" s="10" t="s">
         <v>130</v>
@@ -1955,16 +2021,16 @@
         <v>123</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H10" s="9">
         <v>8</v>
@@ -1973,7 +2039,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>20</v>
@@ -1999,7 +2065,7 @@
         <v>128</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="U10" s="10" t="s">
         <v>130</v>
@@ -2016,16 +2082,16 @@
         <v>123</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H11" s="9">
         <v>9</v>
@@ -2034,7 +2100,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>20</v>
@@ -2060,7 +2126,7 @@
         <v>128</v>
       </c>
       <c r="T11" s="12" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="U11" s="10" t="s">
         <v>130</v>
@@ -2077,16 +2143,16 @@
         <v>123</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H12" s="9">
         <v>10</v>
@@ -2095,7 +2161,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>20</v>
@@ -2121,186 +2187,184 @@
         <v>128</v>
       </c>
       <c r="T12" s="12" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="U12" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:21" s="51" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="F13" s="9" t="s">
+      <c r="D13" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="F13" s="41"/>
+      <c r="G13" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="H13" s="41">
+        <v>11</v>
+      </c>
+      <c r="I13" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="K13" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="R13" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="S13" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="T13" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="U13" s="48" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="55" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53" t="s">
+        <v>161</v>
+      </c>
+      <c r="G14" s="53" t="s">
         <v>164</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="H14" s="53">
+        <v>12</v>
+      </c>
+      <c r="I14" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="53" t="s">
+        <v>165</v>
+      </c>
+      <c r="K14" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
+      <c r="O14" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="P14" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14" s="53" t="s">
+        <v>166</v>
+      </c>
+      <c r="R14" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="H13" s="9">
-        <v>11</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="17" t="s">
+      <c r="S14" s="53" t="s">
         <v>168</v>
       </c>
-      <c r="K13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="P13" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q13" s="10" t="s">
+      <c r="T14" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="R13" s="11" t="s">
+      <c r="U14" s="53" t="s">
         <v>170</v>
-      </c>
-      <c r="S13" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="T13" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="U13" s="10" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="H14" s="9">
-        <v>12</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="R14" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="S14" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="T14" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="U14" s="10" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="H15" s="9">
+      <c r="D15" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="H15" s="23">
         <v>13</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="K15" s="7" t="s">
+      <c r="J15" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="K15" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="L15" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8" t="s">
+      <c r="M15" s="22"/>
+      <c r="N15" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9" t="s">
+      <c r="O15" s="23"/>
+      <c r="P15" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="10">
+      <c r="Q15" s="34">
         <v>6</v>
       </c>
-      <c r="R15" s="11" t="s">
+      <c r="R15" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="S15" s="10" t="s">
+      <c r="S15" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="T15" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="U15" s="10" t="s">
+      <c r="T15" s="36" t="s">
+        <v>197</v>
+      </c>
+      <c r="U15" s="34" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2315,34 +2379,34 @@
         <v>123</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="16" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H16" s="9">
         <v>14</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="N16" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="O16" s="9"/>
       <c r="P16" s="9" t="s">
         <v>19</v>
@@ -2351,75 +2415,77 @@
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>182</v>
+        <v>128</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" s="55" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="53" t="s">
         <v>122</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="D17" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="H17" s="9">
+      <c r="D17" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="G17" s="53" t="s">
+        <v>190</v>
+      </c>
+      <c r="H17" s="53">
         <v>15</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9" t="s">
+      <c r="I17" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="10">
-        <v>6</v>
-      </c>
-      <c r="R17" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="S17" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="T17" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="U17" s="10" t="s">
-        <v>130</v>
+      <c r="J17" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="K17" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="M17" s="54"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="P17" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="R17" s="53" t="s">
+        <v>140</v>
+      </c>
+      <c r="S17" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="T17" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="U17" s="53" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -2433,14 +2499,14 @@
         <v>123</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H18" s="9">
         <v>16</v>
@@ -2449,7 +2515,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2475,7 +2541,7 @@
         <v>128</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="U18" s="10" t="s">
         <v>130</v>
@@ -2492,14 +2558,14 @@
         <v>123</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F19" s="9"/>
-      <c r="G19" s="16" t="s">
-        <v>191</v>
+      <c r="G19" s="57" t="s">
+        <v>234</v>
       </c>
       <c r="H19" s="9">
         <v>17</v>
@@ -2507,8 +2573,8 @@
       <c r="I19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="17" t="s">
-        <v>192</v>
+      <c r="J19" s="56" t="s">
+        <v>233</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2534,7 +2600,7 @@
         <v>128</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="U19" s="10" t="s">
         <v>130</v>
@@ -2552,174 +2618,170 @@
         <v>123</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E20" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G20" s="16" t="s">
         <v>193</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>195</v>
       </c>
       <c r="H20" s="9">
         <v>18</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="9" t="s">
-        <v>138</v>
-      </c>
+      <c r="N20" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="O20" s="9"/>
       <c r="P20" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="10" t="s">
+      <c r="Q20" s="10">
+        <v>6</v>
+      </c>
+      <c r="R20" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="S20" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="T20" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="U20" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" s="51" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="F21" s="41"/>
+      <c r="G21" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="H21" s="41">
+        <v>19</v>
+      </c>
+      <c r="I21" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="44" t="s">
+        <v>202</v>
+      </c>
+      <c r="K21" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="P21" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="R20" s="11" t="s">
+      <c r="R21" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="S20" s="10" t="s">
+      <c r="S21" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="T20" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="U20" s="10" t="s">
+      <c r="T21" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="U21" s="48" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+    <row r="22" spans="1:22" s="55" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B22" s="58" t="s">
         <v>122</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C22" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D22" s="58" t="s">
         <v>204</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="G21" s="16" t="s">
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="H22" s="58">
+        <v>20</v>
+      </c>
+      <c r="I22" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="K22" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="M22" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="N22" s="52"/>
+      <c r="O22" s="58"/>
+      <c r="P22" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q22" s="58">
+        <v>6</v>
+      </c>
+      <c r="R22" s="58" t="s">
+        <v>178</v>
+      </c>
+      <c r="S22" s="58" t="s">
+        <v>179</v>
+      </c>
+      <c r="T22" s="58" t="s">
         <v>198</v>
       </c>
-      <c r="H21" s="9">
-        <v>19</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q21" s="10">
-        <v>6</v>
-      </c>
-      <c r="R21" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="S21" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="T21" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="U21" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="H22" s="9">
-        <v>20</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="P22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q22" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="R22" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="S22" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="T22" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="U22" s="10" t="s">
-        <v>143</v>
+      <c r="U22" s="58" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -2733,14 +2795,14 @@
         <v>123</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="16" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H23" s="9">
         <v>21</v>
@@ -2749,7 +2811,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>20</v>
@@ -2775,7 +2837,7 @@
         <v>128</v>
       </c>
       <c r="T23" s="12" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="U23" s="10" t="s">
         <v>130</v>
@@ -2792,14 +2854,14 @@
         <v>123</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="16" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="H24" s="9">
         <v>22</v>
@@ -2808,7 +2870,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>19</v>
@@ -2832,123 +2894,123 @@
         <v>141</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="U24" s="10" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
+    <row r="25" spans="1:22" s="51" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="H25" s="9">
+      <c r="D25" s="40" t="s">
+        <v>204</v>
+      </c>
+      <c r="E25" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="F25" s="41"/>
+      <c r="G25" s="42" t="s">
+        <v>212</v>
+      </c>
+      <c r="H25" s="41">
         <v>23</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="I25" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="K25" s="7" t="s">
+      <c r="J25" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="K25" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L25" s="6" t="s">
+      <c r="L25" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8" t="s">
+      <c r="M25" s="47"/>
+      <c r="N25" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9" t="s">
+      <c r="O25" s="41"/>
+      <c r="P25" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" s="10">
+      <c r="Q25" s="48">
         <v>6</v>
       </c>
-      <c r="R25" s="11" t="s">
+      <c r="R25" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="S25" s="10" t="s">
+      <c r="S25" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="T25" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="U25" s="10" t="s">
+      <c r="T25" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="U25" s="48" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="H26" s="9">
+      <c r="D26" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="E26" s="29"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="H26" s="23">
         <v>24</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="K26" s="7" t="s">
+      <c r="J26" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="K26" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="L26" s="6" t="s">
+      <c r="L26" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9" t="s">
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="R26" s="11" t="s">
+      <c r="Q26" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="R26" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="S26" s="10" t="s">
+      <c r="S26" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="T26" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="U26" s="10" t="s">
+      <c r="T26" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="U26" s="34" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2963,12 +3025,12 @@
         <v>123</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E27" s="13"/>
       <c r="F27" s="9"/>
       <c r="G27" s="16" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="H27" s="9">
         <v>25</v>
@@ -2977,7 +3039,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>20</v>
@@ -3003,7 +3065,7 @@
         <v>128</v>
       </c>
       <c r="T27" s="12" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="U27" s="10" t="s">
         <v>130</v>
@@ -3020,12 +3082,12 @@
         <v>123</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="9"/>
       <c r="G28" s="16" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="H28" s="9">
         <v>26</v>
@@ -3034,7 +3096,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>20</v>
@@ -3065,12 +3127,12 @@
         <v>123</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="9"/>
       <c r="G29" s="16" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="H29" s="9">
         <v>27</v>
@@ -3079,7 +3141,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>20</v>
@@ -3105,7 +3167,7 @@
         <v>128</v>
       </c>
       <c r="T29" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="U29" s="10" t="s">
         <v>130</v>
@@ -3122,12 +3184,12 @@
         <v>123</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="9"/>
       <c r="G30" s="16" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="H30" s="9">
         <v>28</v>
@@ -3136,7 +3198,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>20</v>
@@ -3162,7 +3224,7 @@
         <v>128</v>
       </c>
       <c r="T30" s="12" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="U30" s="10" t="s">
         <v>130</v>
@@ -4496,7 +4558,14 @@
     <row r="285" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <autoFilter ref="M2:N30"/>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4511,12 +4580,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4527,37 +4590,37 @@
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>P3:P4 I3:I72 K3:K72 P6:P72</xm:sqref>
+          <xm:sqref>P4:P22 P23:P72 K3:K22 K23:K72 I3:I22 I23:I72</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[1]DATOS!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>P5</xm:sqref>
+          <xm:sqref>P3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N72</xm:sqref>
+          <xm:sqref>N3:N22 N23:N72</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A72</xm:sqref>
+          <xm:sqref>A3:A22 A23:A72</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L72</xm:sqref>
+          <xm:sqref>L3:L22 L23:L72</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$1:$E$13</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M72</xm:sqref>
+          <xm:sqref>M3:M22 M23:M72</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>